<commit_message>
on clicking emp details we see two buttons
</commit_message>
<xml_diff>
--- a/Employee_details.xlsx
+++ b/Employee_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Divya\Programming\Python pgrms\Online_course_pgms\Automation_programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DBFE4F-0C03-47A8-9460-EFDFF77967C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6029D9-85F8-4D9C-AE80-21705C0DAA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{88ECCDFA-8245-420E-B59B-C7DC02694C02}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>TEAM</t>
-  </si>
-  <si>
-    <t>USERNAME</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>MANAGER</t>
   </si>
@@ -39,16 +33,22 @@
     <t>Divya</t>
   </si>
   <si>
-    <t>Shubh</t>
-  </si>
-  <si>
     <t>Ridhima</t>
   </si>
   <si>
-    <t>Technical</t>
-  </si>
-  <si>
-    <t>Accounts</t>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Shubham</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D612AF5A-ECCC-4A51-9B31-06F8F6479E65}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -408,40 +408,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="3" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>